<commit_message>
excel shit partly done
</commit_message>
<xml_diff>
--- a/newhdfcDetails.xlsx
+++ b/newhdfcDetails.xlsx
@@ -2,12 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="HDFC Bank INFINIA Credit Card Metal Edition" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="HDFC Bank INFINIA Credit Card Metal Edition" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="HDFC Bank Diners Club Black Credit Card" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -62,7 +63,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,6 +426,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -543,102 +562,335 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HDFC Bank Regalia Credit Card</t>
+          <t>HDFC Bank INFINIA Credit Card Metal Edition</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Travel | Shopping</t>
+          <t>Travel | Dining</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Rs. 2,500 (plus applicable taxes)</t>
+          <t>Rs. 12,500 + applicable taxes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rs. 2,500 (plus applicable taxes)</t>
+          <t>Rs. 12,500 + applicable taxes</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,500 bonus Reward points</t>
+          <t>Welcome bonus of 12,500 Reward Points and complimentary Club Marriott membership for the first year.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4 reward points every time one spends Rs. 150.</t>
+          <t>5 Reward Points on every retail spend of Rs. 150,  reward rate of up to 3.3%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Complimentary Domestic and International Lounge Access. You get complimentary travel insurance as well.</t>
+          <t>Complimentary Priority Pass membership with unlimited free access to airport lounges and with Infinia Credit Card Lounge Access Program along with complimentary Club Marriott membership for 1 year, complimentary 2 + 1 night stay at several premium ITC hotels</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>12 free airport lounge access per year within India.</t>
+          <t>Unlimited complimentary access to domestic lounges with the Priority Pass membership for primary as well as add-on Infinia cardholders, unlimited free domestic lounge visits per quarter with Visa/MasterCard domestic lounge program</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Insurance cover worth Rs. 1 Crore against accidental air death and coverage of up to Rs. 15 lakhs against emergency hospitalization for overseas treatment.</t>
+          <t>Insurance cover worth Rs. 3 crore against accidental air death (applicable only in case of death due to an air accident), a cover worth Rs. 50 lakh against medical emergencies during international air travel, Credit shield cover worth Rs. 9 lakh (the outstanding amount on the card is covered in case of accidental death or permanent disability of the primary cardholder).</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Exclusive dine-out passport membership, 5% off additionally, and early access to several festivals &amp; events.</t>
+          <t>Exclusive dining privileges with the Good Food Trail Program and free Club Marriott membership, 1 + 1 complimentary buffet at ITC hotels.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1 RP = Rs. 0.5 for redemption against flights and hotel bookings on HDFC Smartbuy website, 1 RP = up to Rs. 0.35 if you want to redeem against vouchers and poducts, 1 RP = Rs 0.20 for cash back, and Air miles conversion at a value of 1RP = 0.5 air mile.</t>
+          <t>RPs can be redeemed for flight and hotel bookings via SmartBuy (1 RP = Re. 1), Airmiles through net banking (1 RP = 1 Airmile), products and vouchers via net banking or SmartBuy (1 RP = Rs. 0.50), Apple and Tanishq vouchers (1 RP = Re. 1) cashback (1 RP = Rs. 0.30)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Unlimited complimentary golf games at leading golf courses across India and abroad</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>6 airport lounge access every year outside India through the priority pass.</t>
+          <t>Unlimited free access to international lounges across the globe for the primary cardmember and all add-on cardholders.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>You get zero liability protection cover up to Rs 9 lacs in case of misuse or loss of card.</t>
+          <t>In case the card is lost, if you report the same within 24 hours, you have zero cost liability on any fraudulent transaction made with your credit card. Bank not liable for any fraudulent transaction made prior to the time of reporting.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Get the annual fee waived off (second-year onwards) by spending more than 3 lakh in the previous year.</t>
+          <t>Get renewal fee waived by spending Rs. 10 lakh in the previous year.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Rs 99 (plus applicable taxes)</t>
+          <t>Nil</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2% on all foreign currency transactions.</t>
+          <t>2% of the total transaction amount + taxes</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>3.6% per month or 43.2% annually</t>
+          <t>1.99% per month or 23.8% annualized</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>1% fuel surcharge waiver at all fuel stations in India on a minimum of Rs. 400 transaction and a maximum of Rs. 5000 transaction.</t>
+          <t>1% fuel surcharge waiver up to Rs. 1,000 each month</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>2.5% of the transaction amount or Rs. 500 (whichever is higher)</t>
+          <t>NIL (Interests charges applicable)</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Joining Fee</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Renewal Fee</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Welcome Bonus</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Reward Rates</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>travel</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Domestic Lounge Access</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Insurance Benefits</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Movie &amp; Dining</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Reward redemption</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Golf</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>International lounge access</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Zero Liability Protection</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Spend based waiver</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Reward redemption fee</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Foreign currency markup</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Interest Rates</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Fuel Surcharge</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Cash advance charge</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Add on card fee</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HDFC Bank Diners Club Black Credit Card</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Travel | Dining | Shopping</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rs. 10,000 (plus applicable taxes)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Rs. 10,000 (plus applicable taxes)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Complimentary memberships for a year to MMTDOUBLEBLACK, Zomato Gold, Club Marriott, Times Prime, and Amazon Prime.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5 Reward Points for every Rs. 150 spent, accelerated Reward Points while spending on SmartBuy</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Complimentary lounge access at 1,000+ airports in India and abroad, Reward Points redeemable for flight and hotel bookings on SmartBuy (1RP = Re. 1).</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Unlimited complimentary access to the domestic lounges</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Travel-related insurance benefits including an air accident cover worth Rs. 2 crores and a credit liability cover worth up to Rs. 9 lakh.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2X Reward Points on weekend dining, complimentary annual membership of Zomato Gold.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>HDFC Bank Diners Club Black Reward Points are redeemable for flight/hotel bookings (1 RP = Re. 1) on SmartBuy, for AirMiles (1 RP = 1 AirMile), on Diners Club exclusive rewards redemption catalog (1 RP = Re. 0.5) and for cashbacks (1RP = Rs. 0.30).</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>6 complimentary golf games per quarter at some of the most premium golf destinations around the world.</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Unlimited complimentary access to the international lounges</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Zero liability protection worth Rs. 9 lakh against a lost/stolen card.</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Waiver of renewal fee on spending Rs. 5,00,000 in the previous year.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.99% (plus applicable taxes)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1.99% per month (or 23.88% annually)</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>1% fuel surcharge waived (max waiver capped at Rs. 1,000/month and min transaction of  Rs. 400 required).</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Higher of 2.5% of the amount withdrawn or Rs. 500.</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">

</xml_diff>